<commit_message>
Comment style, Add Image
</commit_message>
<xml_diff>
--- a/public/rascal_data.xlsx
+++ b/public/rascal_data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="195">
   <si>
     <t>◎ 라스칼 통산 성적</t>
   </si>
@@ -330,20 +330,20 @@
   </si>
   <si>
     <t>포수 포지션 경쟁 끝에 새로운 집을 짓기로 한 비버마스터
-아이쿠, 이미 1루에 자리잡으려는 세력들이 있군요.
-탄탄한 집을 짓는 비버들과 외야에서 쫒겨나 흉폭한 비버까지...
-비버마스터 혁진권은 이번에야말로 
-자신의 베이스캠프를 완성할 수 있을까요?</t>
+    아이쿠, 이미 1루에 자리잡으려는 세력들이 있군요.
+    탄탄한 집을 짓는 비버들과 외야에서 쫒겨나 흉폭한 비버까지...
+    비버마스터 혁진권은 이번에야말로🌲
+    🌴자신의 베이스캠프를 완성할 수 있을까요?</t>
   </si>
   <si>
     <t>GiBeaver</t>
   </si>
   <si>
-    <t>[{"fontFamily": "Dongle"}, 
-{"fontFamily": "Dongle"},
-{"fontFamily": "Dongle"},
-{"fontFamily": "Dongle"},
-{"fontFamily": "Dongle"}]</t>
+    <t>[{"fontFamily": "Dongle", "fontSize": "17px"}, 
+    {"fontFamily": "Dongle", "fontSize": "18px"},
+    {"fontFamily": "Dongle", "fontSize": "15px"},
+    {"fontFamily": "Dongle", "fontSize": "19px"},
+    {"fontFamily": "Dongle", "fontSize": "19px", "textAlign": "right"}]</t>
   </si>
   <si>
     <r>
@@ -415,7 +415,8 @@
         <color theme="1"/>
         <sz val="10.0"/>
       </rPr>
-      <t>술은 김기태를 상대로 시즌 2승을 올립니다.
+      <t>김기태 선수는 술을 이길 수 없습니다.
+ 시즌 2패.
 연패의 늪에 빠져 정신없이 전화를 돌리는 김기태.</t>
     </r>
   </si>
@@ -540,9 +541,8 @@
         <sz val="11.0"/>
       </rPr>
       <t xml:space="preserve">2023년은 라스칼의 선봉대장 김재영의 해였습니다.
-1번타자 - 타율 1위 , 출루율 1위,
-도루 1위, 득점 1위, V.C 1위
-축하합니다.
+1번타자로 주로 출전 
+타율 1위 , 출루율 1위, 도루 1위, 득점 1위, V.C 1위
 2023년 Rascal MVP는 김재영 선수입니다.
 </t>
     </r>
@@ -578,19 +578,11 @@
         <color theme="1"/>
         <sz val="8.0"/>
       </rPr>
-      <t xml:space="preserve">-2024년에도 총무 연임 확정-
+      <t>-2024년에도 총무 연임 확정-
+-울산으로 이직 성공-
 -전율의 개인커리어 14연패-
 -사진만 찍으면 도형으로 변하는 입-
--역대급 패배요정-
-</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <color theme="1"/>
-        <sz val="7.0"/>
-      </rPr>
-      <t>(개인 커리어 14연패)</t>
+-역대급 패배요정-</t>
     </r>
   </si>
   <si>
@@ -617,8 +609,8 @@
     <t>DongleDongle</t>
   </si>
   <si>
-    <t>언제나 눈부신 태양이지만 그런 태양에게도 흑점이 있듯.
-파이팅 넘치는 그의 이면에는 아티스트의 고뇌와 섬세함이 함께합니다.
+    <t>언제나 눈부신 태양이지만 그런 태양에게도 흑점이 있습니다.
+파이팅 넘치는 태양이의 이면에는 아티스트의 섬세함이 공존합니다.
 가끔 모두의 관심이 부담이되더라도.
 라스칼의 모두가 당신을 좋아하고, 필요로 한다는 것은 꼭 알아주세요. 
 "태양아 기태도 네 실수가 아쉬워서 그러는거지 진심으로 화내는게 아니야."
@@ -708,7 +700,7 @@
         <color theme="1"/>
         <sz val="12.0"/>
       </rPr>
-      <t>"대구에도 주야 2교대는 실존한다!!!!!"</t>
+      <t>"주야 2교대는 실존한다!!!!!"</t>
     </r>
     <r>
       <rPr>
@@ -842,7 +834,16 @@
     <t>3B</t>
   </si>
   <si>
-    <t>MZ</t>
+    <t>매직스틱</t>
+  </si>
+  <si>
+    <t>올시즌 박재현 선수는 그야말로 "용두사미" 였습니다.
+발은 느리지만 볼 컨택 능력을 인정받아 스타팅으로 자리잡으며
+시즌 초중반 박재현 선수는 무서운 타격 퍼포먼스를 선보였습니다.
+그러나 단점인  수비 능력이 성장하지 못하고 스윙 마저 무뎌지면서
+치솟는 삼진율과 함께 스타팅 자리를 내어주며 시즌을 마감합니다.
+포지션 이해도를 높여서 빠른 판단으로 느린 발과 수비를 커버한다면
+24년 가장 강력한 승리 공식이 될 것이라 믿어의심치 않습니다.</t>
   </si>
   <si>
     <t>BAEK JEONG CHEOL</t>
@@ -906,19 +907,31 @@
     <t>LEE DONG JIN</t>
   </si>
   <si>
+    <t>허수아비</t>
+  </si>
+  <si>
     <t>LEE CHEOL MIN</t>
   </si>
   <si>
-    <t>스태프</t>
+    <t>철자후</t>
   </si>
   <si>
     <t>LIM JI HEON</t>
   </si>
   <si>
+    <t>과거의영광</t>
+  </si>
+  <si>
     <t>CHO TAE HYEONG</t>
   </si>
   <si>
+    <t>먹튀</t>
+  </si>
+  <si>
     <t>CHA HYUN CHUL</t>
+  </si>
+  <si>
+    <t>맏형</t>
   </si>
   <si>
     <t>◎ 22년 하반기 드림즈리그</t>
@@ -1534,11 +1547,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1167387808"/>
-        <c:axId val="425007504"/>
+        <c:axId val="586995968"/>
+        <c:axId val="957297444"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1167387808"/>
+        <c:axId val="586995968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1590,10 +1603,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="425007504"/>
+        <c:crossAx val="957297444"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="425007504"/>
+        <c:axId val="957297444"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1657,7 +1670,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1167387808"/>
+        <c:crossAx val="586995968"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1889,11 +1902,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="705244657"/>
-        <c:axId val="485242283"/>
+        <c:axId val="1317401029"/>
+        <c:axId val="1421918952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="705244657"/>
+        <c:axId val="1317401029"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1945,10 +1958,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="485242283"/>
+        <c:crossAx val="1421918952"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="485242283"/>
+        <c:axId val="1421918952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2012,7 +2025,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="705244657"/>
+        <c:crossAx val="1317401029"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2244,11 +2257,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="26227891"/>
-        <c:axId val="1314554326"/>
+        <c:axId val="1403287857"/>
+        <c:axId val="210227726"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="26227891"/>
+        <c:axId val="1403287857"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2300,10 +2313,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1314554326"/>
+        <c:crossAx val="210227726"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1314554326"/>
+        <c:axId val="210227726"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2367,7 +2380,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="26227891"/>
+        <c:crossAx val="1403287857"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2639,11 +2652,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="307517368"/>
-        <c:axId val="1784310262"/>
+        <c:axId val="2006494188"/>
+        <c:axId val="1165119829"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="307517368"/>
+        <c:axId val="2006494188"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2695,10 +2708,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1784310262"/>
+        <c:crossAx val="1165119829"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1784310262"/>
+        <c:axId val="1165119829"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2762,7 +2775,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="307517368"/>
+        <c:crossAx val="2006494188"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2863,11 +2876,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="735992803"/>
-        <c:axId val="1245413842"/>
+        <c:axId val="1408497789"/>
+        <c:axId val="615330453"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="735992803"/>
+        <c:axId val="1408497789"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2919,10 +2932,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1245413842"/>
+        <c:crossAx val="615330453"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1245413842"/>
+        <c:axId val="615330453"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -2987,7 +3000,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="735992803"/>
+        <c:crossAx val="1408497789"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="0"/>
@@ -4736,7 +4749,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
@@ -4746,10 +4759,10 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>33</v>
@@ -5730,10 +5743,10 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>46</v>
@@ -5742,7 +5755,7 @@
         <v>47</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>49</v>
@@ -5772,7 +5785,7 @@
         <v>56</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="P28" s="3" t="s">
         <v>58</v>
@@ -14915,7 +14928,7 @@
     <col customWidth="1" min="6" max="6" width="20.29"/>
     <col customWidth="1" min="7" max="7" width="57.14"/>
     <col customWidth="1" min="8" max="8" width="8.86"/>
-    <col customWidth="1" min="9" max="9" width="76.0"/>
+    <col customWidth="1" min="9" max="9" width="68.71"/>
     <col customWidth="1" min="10" max="10" width="45.43"/>
     <col customWidth="1" min="11" max="11" width="19.29"/>
   </cols>
@@ -15433,7 +15446,7 @@
         <v>162</v>
       </c>
       <c r="F16" s="39">
-        <v>30.0</v>
+        <v>12.11</v>
       </c>
       <c r="G16" s="58" t="s">
         <v>163</v>
@@ -15467,9 +15480,11 @@
         <v>168</v>
       </c>
       <c r="F17" s="39">
-        <v>1.0</v>
-      </c>
-      <c r="G17" s="43"/>
+        <v>100.0</v>
+      </c>
+      <c r="G17" s="40" t="s">
+        <v>169</v>
+      </c>
       <c r="H17" s="56"/>
       <c r="I17" s="43"/>
       <c r="J17" s="43"/>
@@ -15478,7 +15493,7 @@
     </row>
     <row r="18">
       <c r="A18" s="37" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B18" s="38" t="s">
         <v>23</v>
@@ -15490,31 +15505,31 @@
         <v>107</v>
       </c>
       <c r="E18" s="39" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F18" s="39">
         <v>100.0</v>
       </c>
       <c r="G18" s="49" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H18" s="47" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I18" s="44" t="s">
         <v>125</v>
       </c>
       <c r="J18" s="46" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="K18" s="43"/>
       <c r="L18" s="58" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="37" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B19" s="38" t="s">
         <v>24</v>
@@ -15525,9 +15540,11 @@
       <c r="D19" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="E19" s="57"/>
+      <c r="E19" s="39" t="s">
+        <v>177</v>
+      </c>
       <c r="F19" s="39">
-        <v>50.0</v>
+        <v>15.0</v>
       </c>
       <c r="G19" s="43"/>
       <c r="H19" s="56"/>
@@ -15538,7 +15555,7 @@
     </row>
     <row r="20">
       <c r="A20" s="37" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B20" s="38" t="s">
         <v>25</v>
@@ -15550,7 +15567,7 @@
         <v>100</v>
       </c>
       <c r="E20" s="39" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F20" s="39">
         <v>100.0</v>
@@ -15564,7 +15581,7 @@
     </row>
     <row r="21">
       <c r="A21" s="37" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B21" s="38" t="s">
         <v>26</v>
@@ -15575,9 +15592,8 @@
       <c r="D21" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="E21" s="57" t="str">
-        <f t="shared" ref="E21:E23" si="2">RIGHT(B21,LEN(B21) - 1)</f>
-        <v>지헌</v>
+      <c r="E21" s="39" t="s">
+        <v>181</v>
       </c>
       <c r="F21" s="39">
         <v>50.0</v>
@@ -15591,7 +15607,7 @@
     </row>
     <row r="22">
       <c r="A22" s="37" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B22" s="38" t="s">
         <v>27</v>
@@ -15602,9 +15618,8 @@
       <c r="D22" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="E22" s="57" t="str">
-        <f t="shared" si="2"/>
-        <v>태형</v>
+      <c r="E22" s="39" t="s">
+        <v>183</v>
       </c>
       <c r="F22" s="39">
         <v>50.0</v>
@@ -15618,7 +15633,7 @@
     </row>
     <row r="23">
       <c r="A23" s="37" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="B23" s="38" t="s">
         <v>28</v>
@@ -15627,9 +15642,8 @@
         <v>20.0</v>
       </c>
       <c r="D23" s="38"/>
-      <c r="E23" s="57" t="str">
-        <f t="shared" si="2"/>
-        <v>현철</v>
+      <c r="E23" s="60" t="s">
+        <v>185</v>
       </c>
       <c r="F23" s="39">
         <v>50.0</v>
@@ -15668,7 +15682,7 @@
   <sheetData>
     <row r="1" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" ht="16.5" customHeight="1">
@@ -18066,7 +18080,7 @@
   <sheetData>
     <row r="1" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="B1" s="64"/>
       <c r="C1" s="64"/>
@@ -18118,10 +18132,10 @@
     </row>
     <row r="3" ht="16.5" customHeight="1">
       <c r="A3" s="67" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B3" s="67" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C3" s="67" t="s">
         <v>33</v>
@@ -19070,10 +19084,10 @@
     </row>
     <row r="28" ht="16.5" customHeight="1">
       <c r="A28" s="67" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B28" s="67" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C28" s="67" t="s">
         <v>46</v>
@@ -19100,10 +19114,10 @@
         <v>52</v>
       </c>
       <c r="K28" s="67" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="L28" s="67" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="M28" s="67" t="s">
         <v>41</v>
@@ -19112,7 +19126,7 @@
         <v>56</v>
       </c>
       <c r="O28" s="67" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="P28" s="67" t="s">
         <v>58</v>

</xml_diff>